<commit_message>
Excel up and running
</commit_message>
<xml_diff>
--- a/backend/Customer Emails.xlsx
+++ b/backend/Customer Emails.xlsx
@@ -7,7 +7,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Customers" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Customers1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -371,7 +370,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,39 +390,52 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Tester One</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dbctesteremail@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Tester Two</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>soxreceiveremail@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tester Three</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>soxreceiver2email@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Tester One</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>soxreceiver@gmail.com</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>